<commit_message>
Ajout du dossier de projet
Ajout du dossier de projet DMS-SHOES
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravailEtBordDMS_SimaoHenriquesDaSilva.xlsx
+++ b/Documentation/JournalDeTravailEtBordDMS_SimaoHenriquesDaSilva.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\2eme annee\ProjetWeb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simao.HENRIQUES-SILV\Documents\GitHub\ProjetWebDMS\ProjetWebDMS\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
   <si>
     <t>Nom du Projet :</t>
   </si>
@@ -145,6 +145,21 @@
   </si>
   <si>
     <t>Remplissage du Journal de travail avec ce qui déjà été fait</t>
+  </si>
+  <si>
+    <t>Commencement du Dossier de projet</t>
+  </si>
+  <si>
+    <t>Commencement du dossier de projet DMS-SHOES</t>
+  </si>
+  <si>
+    <t>Continuation du Dossier de projet</t>
+  </si>
+  <si>
+    <t>Continuation du Dossier de projet DMS-SHOES</t>
+  </si>
+  <si>
+    <t>Simão Henirques da Silva</t>
   </si>
 </sst>
 </file>
@@ -695,40 +710,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -755,7 +743,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -1362,8 +1377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N9999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,27 +1400,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
     </row>
     <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.25">
       <c r="F2" s="17"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
     </row>
     <row r="3" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F3" s="18"/>
@@ -1413,14 +1428,14 @@
       <c r="H3" s="18"/>
     </row>
     <row r="4" spans="2:14" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="48" t="s">
+      <c r="C4" s="34"/>
+      <c r="D4" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="49"/>
+      <c r="E4" s="40"/>
       <c r="G4" s="20" t="s">
         <v>1</v>
       </c>
@@ -1447,14 +1462,14 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="46" t="s">
+      <c r="C5" s="32"/>
+      <c r="D5" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="47"/>
+      <c r="E5" s="38"/>
       <c r="G5" s="4">
         <v>44957</v>
       </c>
@@ -1482,14 +1497,14 @@
       </c>
     </row>
     <row r="6" spans="2:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="44">
+      <c r="C6" s="32"/>
+      <c r="D6" s="35">
         <v>44957</v>
       </c>
-      <c r="E6" s="45"/>
+      <c r="E6" s="36"/>
       <c r="G6" s="4">
         <v>44957</v>
       </c>
@@ -1517,15 +1532,15 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="40">
+      <c r="C7" s="48"/>
+      <c r="D7" s="49">
         <f>SUM(Tableau1[Durée])</f>
-        <v>0.17222222222222261</v>
+        <v>0.23472222222222261</v>
       </c>
-      <c r="E7" s="41"/>
+      <c r="E7" s="50"/>
       <c r="G7" s="4">
         <v>44957</v>
       </c>
@@ -1581,10 +1596,10 @@
     </row>
     <row r="9" spans="2:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="16"/>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="31"/>
+      <c r="D9" s="42"/>
       <c r="G9" s="4">
         <v>44959</v>
       </c>
@@ -1615,10 +1630,10 @@
       <c r="B10" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="33"/>
+      <c r="D10" s="44"/>
       <c r="G10" s="4">
         <v>44959</v>
       </c>
@@ -1649,10 +1664,10 @@
       <c r="B11" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="35"/>
+      <c r="D11" s="46"/>
       <c r="G11" s="4">
         <v>44959</v>
       </c>
@@ -1679,31 +1694,59 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="G12" s="4"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="6"/>
+    <row r="12" spans="2:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="G12" s="4">
+        <v>44959</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0.70486111111111116</v>
+      </c>
       <c r="J12" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
-      <c r="K12" s="7"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="G13" s="4"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="6"/>
+      <c r="K12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="G13" s="4">
+        <v>44960</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="I13" s="6">
+        <v>0.70486111111111116</v>
+      </c>
       <c r="J13" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
-      <c r="K13" s="7"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
+      <c r="K13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="G14" s="4"/>
@@ -44225,18 +44268,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D7:E7"/>
     <mergeCell ref="G1:N2"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D4:E4"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1"/>
@@ -44597,9 +44640,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -44773,26 +44819,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D38AEF9-57C3-439A-B892-EB0F14AB4CC0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE66B988-21FD-4E82-857E-C2E9A6618F3F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="9b42e094-9454-4e38-a519-f9a276a20d04"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -44816,9 +44851,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE66B988-21FD-4E82-857E-C2E9A6618F3F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D38AEF9-57C3-439A-B892-EB0F14AB4CC0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="9b42e094-9454-4e38-a519-f9a276a20d04"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Mise à jour du Journal de Bord
Mise à jour du Journal de Bord avec la modification du dossier de projet et de la modification du cahier des charges
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravailEtBordDMS_SimaoHenriquesDaSilva.xlsx
+++ b/Documentation/JournalDeTravailEtBordDMS_SimaoHenriquesDaSilva.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
   <si>
     <t>Nom du Projet :</t>
   </si>
@@ -166,6 +166,15 @@
   </si>
   <si>
     <t>Ajout des zooning dans le Dossier de Projet</t>
+  </si>
+  <si>
+    <t>Prise de tâche sur IceScrum</t>
+  </si>
+  <si>
+    <t>Prise de tâche sur IceScrum et fin des tâches</t>
+  </si>
+  <si>
+    <t>Mise à jour du dossier de projet et du cahier des charges</t>
   </si>
 </sst>
 </file>
@@ -716,13 +725,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -748,36 +787,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1383,8 +1392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N9999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1406,27 +1415,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
     </row>
     <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.25">
       <c r="F2" s="17"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
     </row>
     <row r="3" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F3" s="18"/>
@@ -1434,14 +1443,14 @@
       <c r="H3" s="18"/>
     </row>
     <row r="4" spans="2:14" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="39" t="s">
+      <c r="C4" s="44"/>
+      <c r="D4" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="40"/>
+      <c r="E4" s="50"/>
       <c r="G4" s="20" t="s">
         <v>1</v>
       </c>
@@ -1468,14 +1477,14 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="37" t="s">
+      <c r="C5" s="39"/>
+      <c r="D5" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="38"/>
+      <c r="E5" s="48"/>
       <c r="G5" s="4">
         <v>44957</v>
       </c>
@@ -1503,14 +1512,14 @@
       </c>
     </row>
     <row r="6" spans="2:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="35">
+      <c r="C6" s="39"/>
+      <c r="D6" s="45">
         <v>44957</v>
       </c>
-      <c r="E6" s="36"/>
+      <c r="E6" s="46"/>
       <c r="G6" s="4">
         <v>44957</v>
       </c>
@@ -1538,15 +1547,15 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="49">
+      <c r="C7" s="37"/>
+      <c r="D7" s="40">
         <f>SUM(Tableau1[Durée])</f>
-        <v>0.28750000000000042</v>
+        <v>0.29791666666666705</v>
       </c>
-      <c r="E7" s="50"/>
+      <c r="E7" s="41"/>
       <c r="G7" s="4">
         <v>44957</v>
       </c>
@@ -1602,10 +1611,10 @@
     </row>
     <row r="9" spans="2:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="16"/>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="42"/>
+      <c r="D9" s="31"/>
       <c r="G9" s="4">
         <v>44959</v>
       </c>
@@ -1636,10 +1645,10 @@
       <c r="B10" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="44"/>
+      <c r="D10" s="33"/>
       <c r="G10" s="4">
         <v>44959</v>
       </c>
@@ -1670,10 +1679,10 @@
       <c r="B11" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="46"/>
+      <c r="D11" s="35"/>
       <c r="G11" s="4">
         <v>44959</v>
       </c>
@@ -1808,31 +1817,59 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="G16" s="4"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="6"/>
+    <row r="16" spans="2:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="G16" s="4">
+        <v>44966</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="I16" s="6">
+        <v>0.62152777777777779</v>
+      </c>
       <c r="J16" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>0</v>
+        <v>3.4722222222222099E-3</v>
       </c>
-      <c r="K16" s="7"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-    </row>
-    <row r="17" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G17" s="4"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="6"/>
+      <c r="K16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="7:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="G17" s="4">
+        <v>44966</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0.62152777777777779</v>
+      </c>
+      <c r="I17" s="6">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="J17" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>0</v>
+        <v>6.9444444444444198E-3</v>
       </c>
-      <c r="K17" s="7"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
+      <c r="K17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="18" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G18" s="4"/>
@@ -44302,18 +44339,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:N2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D4:E4"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D7:E7"/>
-    <mergeCell ref="G1:N2"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D4:E4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1"/>
@@ -44674,12 +44711,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -44853,15 +44887,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE66B988-21FD-4E82-857E-C2E9A6618F3F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D38AEF9-57C3-439A-B892-EB0F14AB4CC0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="9b42e094-9454-4e38-a519-f9a276a20d04"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -44885,17 +44930,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D38AEF9-57C3-439A-B892-EB0F14AB4CC0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE66B988-21FD-4E82-857E-C2E9A6618F3F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="9b42e094-9454-4e38-a519-f9a276a20d04"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Mise à jour du journal de travail / journal de bord
Mise à jour du journal de travail / journal de bord pour l'ajout de User Story et du retour du cahier des charges.
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravailEtBordDMS_SimaoHenriquesDaSilva.xlsx
+++ b/Documentation/JournalDeTravailEtBordDMS_SimaoHenriquesDaSilva.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="66">
   <si>
     <t>Nom du Projet :</t>
   </si>
@@ -211,6 +211,18 @@
   </si>
   <si>
     <t>Ajout de la template et modification du code</t>
+  </si>
+  <si>
+    <t>Ajout de User story</t>
+  </si>
+  <si>
+    <t>Ajout de plus de User Story pour les prochain sprint</t>
+  </si>
+  <si>
+    <t>Retour du cahier des charges</t>
+  </si>
+  <si>
+    <t>M.MEYLAN</t>
   </si>
 </sst>
 </file>
@@ -680,7 +692,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -758,16 +770,45 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -794,37 +835,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1428,8 +1445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N9999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1451,27 +1468,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
     </row>
     <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.25">
       <c r="F2" s="17"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
     </row>
     <row r="3" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F3" s="18"/>
@@ -1479,14 +1496,14 @@
       <c r="H3" s="18"/>
     </row>
     <row r="4" spans="2:14" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="39" t="s">
+      <c r="C4" s="43"/>
+      <c r="D4" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="40"/>
+      <c r="E4" s="49"/>
       <c r="G4" s="20" t="s">
         <v>1</v>
       </c>
@@ -1513,14 +1530,14 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="37" t="s">
+      <c r="C5" s="38"/>
+      <c r="D5" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="38"/>
+      <c r="E5" s="47"/>
       <c r="G5" s="4">
         <v>44957</v>
       </c>
@@ -1548,14 +1565,14 @@
       </c>
     </row>
     <row r="6" spans="2:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="35">
+      <c r="C6" s="38"/>
+      <c r="D6" s="44">
         <v>44957</v>
       </c>
-      <c r="E6" s="36"/>
+      <c r="E6" s="45"/>
       <c r="G6" s="4">
         <v>44957</v>
       </c>
@@ -1583,15 +1600,15 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="49">
+      <c r="C7" s="36"/>
+      <c r="D7" s="39">
         <f>SUM(Tableau1[Durée])</f>
-        <v>0.44722222222222241</v>
-      </c>
-      <c r="E7" s="50"/>
+        <v>0.47500000000000009</v>
+      </c>
+      <c r="E7" s="40"/>
       <c r="G7" s="4">
         <v>44957</v>
       </c>
@@ -1647,10 +1664,10 @@
     </row>
     <row r="9" spans="2:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="16"/>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="42"/>
+      <c r="D9" s="30"/>
       <c r="G9" s="4">
         <v>44959</v>
       </c>
@@ -1681,10 +1698,10 @@
       <c r="B10" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="44"/>
+      <c r="D10" s="32"/>
       <c r="G10" s="4">
         <v>44959</v>
       </c>
@@ -1715,10 +1732,10 @@
       <c r="B11" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="46"/>
+      <c r="D11" s="34"/>
       <c r="G11" s="4">
         <v>44959</v>
       </c>
@@ -2096,18 +2113,32 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G25" s="4"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="6"/>
+    <row r="25" spans="7:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="G25" s="4">
+        <v>44985</v>
+      </c>
+      <c r="H25" s="5">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="I25" s="6">
+        <v>0.70138888888888884</v>
+      </c>
       <c r="J25" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>0</v>
-      </c>
-      <c r="K25" s="7"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
+        <v>2.7777777777777679E-2</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L25" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="26" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G26" s="4"/>
@@ -44473,18 +44504,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:N2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D4:E4"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D7:E7"/>
-    <mergeCell ref="G1:N2"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D4:E4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1"/>
@@ -44502,23 +44533,23 @@
   <dimension ref="B1:G63"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="45" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
       <c r="G1" s="25"/>
     </row>
     <row r="3" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -44533,304 +44564,310 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
+      <c r="C4" s="52">
+        <v>44981</v>
+      </c>
+      <c r="D4" s="51" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="51" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
     </row>
     <row r="30" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="28"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
     </row>
     <row r="32" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="28"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C36" s="28"/>
-      <c r="D36" s="28"/>
-      <c r="E36" s="28"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="28"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C38" s="28"/>
-      <c r="D38" s="28"/>
-      <c r="E38" s="28"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="28"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="28"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="28"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="28"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="28"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
     </row>
     <row r="44" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="28"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27"/>
     </row>
     <row r="46" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="28"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="27"/>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C47" s="28"/>
-      <c r="D47" s="28"/>
-      <c r="E47" s="28"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
     </row>
     <row r="48" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C48" s="28"/>
-      <c r="D48" s="28"/>
-      <c r="E48" s="28"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27"/>
     </row>
     <row r="49" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C49" s="28"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="28"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="27"/>
     </row>
     <row r="50" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C50" s="28"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="28"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="27"/>
     </row>
     <row r="51" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C51" s="28"/>
-      <c r="D51" s="28"/>
-      <c r="E51" s="28"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="27"/>
     </row>
     <row r="52" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C52" s="28"/>
-      <c r="D52" s="28"/>
-      <c r="E52" s="28"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="27"/>
     </row>
     <row r="53" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C53" s="28"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="28"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="27"/>
     </row>
     <row r="54" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C54" s="28"/>
-      <c r="D54" s="28"/>
-      <c r="E54" s="28"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="27"/>
     </row>
     <row r="55" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C55" s="28"/>
-      <c r="D55" s="28"/>
-      <c r="E55" s="28"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="27"/>
     </row>
     <row r="56" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C56" s="28"/>
-      <c r="D56" s="28"/>
-      <c r="E56" s="28"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="27"/>
+      <c r="E56" s="27"/>
     </row>
     <row r="57" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C57" s="28"/>
-      <c r="D57" s="28"/>
-      <c r="E57" s="28"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="27"/>
     </row>
     <row r="58" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C58" s="28"/>
-      <c r="D58" s="28"/>
-      <c r="E58" s="28"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="27"/>
+      <c r="E58" s="27"/>
     </row>
     <row r="59" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C59" s="28"/>
-      <c r="D59" s="28"/>
-      <c r="E59" s="28"/>
+      <c r="C59" s="27"/>
+      <c r="D59" s="27"/>
+      <c r="E59" s="27"/>
     </row>
     <row r="60" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C60" s="28"/>
-      <c r="D60" s="28"/>
-      <c r="E60" s="28"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="27"/>
+      <c r="E60" s="27"/>
     </row>
     <row r="61" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C61" s="28"/>
-      <c r="D61" s="28"/>
-      <c r="E61" s="28"/>
+      <c r="C61" s="27"/>
+      <c r="D61" s="27"/>
+      <c r="E61" s="27"/>
     </row>
     <row r="62" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C62" s="28"/>
-      <c r="D62" s="28"/>
-      <c r="E62" s="28"/>
+      <c r="C62" s="27"/>
+      <c r="D62" s="27"/>
+      <c r="E62" s="27"/>
     </row>
     <row r="63" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C63" s="29"/>
-      <c r="D63" s="29"/>
-      <c r="E63" s="29"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -44845,12 +44882,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -45024,15 +45058,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE66B988-21FD-4E82-857E-C2E9A6618F3F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D38AEF9-57C3-439A-B892-EB0F14AB4CC0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="9b42e094-9454-4e38-a519-f9a276a20d04"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -45056,17 +45101,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D38AEF9-57C3-439A-B892-EB0F14AB4CC0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE66B988-21FD-4E82-857E-C2E9A6618F3F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="9b42e094-9454-4e38-a519-f9a276a20d04"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Mise a jour du journal de travail
Mise a jour du journal de travail avec l'avancer du login
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravailEtBordDMS_SimaoHenriquesDaSilva.xlsx
+++ b/Documentation/JournalDeTravailEtBordDMS_SimaoHenriquesDaSilva.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="69">
   <si>
     <t>Nom du Projet :</t>
   </si>
@@ -223,6 +223,15 @@
   </si>
   <si>
     <t>M.MEYLAN</t>
+  </si>
+  <si>
+    <t>Code du login</t>
+  </si>
+  <si>
+    <t>Création du code du login / register du site</t>
+  </si>
+  <si>
+    <t>Simão Henriques  da Silva , Marcos Valente da Silva , Diego Pinto Tomaz</t>
   </si>
 </sst>
 </file>
@@ -778,13 +787,43 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -810,36 +849,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1446,7 +1455,7 @@
   <dimension ref="B1:N9999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1468,27 +1477,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
     </row>
     <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.25">
       <c r="F2" s="17"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
     </row>
     <row r="3" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F3" s="18"/>
@@ -1496,14 +1505,14 @@
       <c r="H3" s="18"/>
     </row>
     <row r="4" spans="2:14" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="40" t="s">
+      <c r="C4" s="45"/>
+      <c r="D4" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="41"/>
+      <c r="E4" s="51"/>
       <c r="G4" s="20" t="s">
         <v>1</v>
       </c>
@@ -1530,14 +1539,14 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="38" t="s">
+      <c r="C5" s="40"/>
+      <c r="D5" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="39"/>
+      <c r="E5" s="49"/>
       <c r="G5" s="4">
         <v>44957</v>
       </c>
@@ -1565,14 +1574,14 @@
       </c>
     </row>
     <row r="6" spans="2:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="36">
+      <c r="C6" s="40"/>
+      <c r="D6" s="46">
         <v>44957</v>
       </c>
-      <c r="E6" s="37"/>
+      <c r="E6" s="47"/>
       <c r="G6" s="4">
         <v>44957</v>
       </c>
@@ -1600,15 +1609,15 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="50">
+      <c r="C7" s="38"/>
+      <c r="D7" s="41">
         <f>SUM(Tableau1[Durée])</f>
-        <v>0.5409722222222223</v>
-      </c>
-      <c r="E7" s="51"/>
+        <v>0.60694444444444451</v>
+      </c>
+      <c r="E7" s="42"/>
       <c r="G7" s="4">
         <v>44957</v>
       </c>
@@ -1664,10 +1673,10 @@
     </row>
     <row r="9" spans="2:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="16"/>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="43"/>
+      <c r="D9" s="32"/>
       <c r="G9" s="4">
         <v>44959</v>
       </c>
@@ -1698,10 +1707,10 @@
       <c r="B10" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="45"/>
+      <c r="D10" s="34"/>
       <c r="G10" s="4">
         <v>44959</v>
       </c>
@@ -1732,10 +1741,10 @@
       <c r="B11" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="47"/>
+      <c r="D11" s="36"/>
       <c r="G11" s="4">
         <v>44959</v>
       </c>
@@ -2167,18 +2176,32 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G27" s="4"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="6"/>
+    <row r="27" spans="7:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="G27" s="4">
+        <v>44987</v>
+      </c>
+      <c r="H27" s="5">
+        <v>0.5625</v>
+      </c>
+      <c r="I27" s="6">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="J27" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>0</v>
-      </c>
-      <c r="K27" s="7"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L27" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="28" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G28" s="4"/>
@@ -44518,18 +44541,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:N2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D4:E4"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D7:E7"/>
-    <mergeCell ref="G1:N2"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D4:E4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1"/>
@@ -44896,12 +44919,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -45075,15 +45095,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE66B988-21FD-4E82-857E-C2E9A6618F3F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D38AEF9-57C3-439A-B892-EB0F14AB4CC0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="9b42e094-9454-4e38-a519-f9a276a20d04"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -45107,17 +45138,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D38AEF9-57C3-439A-B892-EB0F14AB4CC0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE66B988-21FD-4E82-857E-C2E9A6618F3F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="9b42e094-9454-4e38-a519-f9a276a20d04"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Mise a jour des journaux de travails
J'ai mis à jour mon journal de travail et Simao a mis a jour son journal de travail jusqu'à le 28.03.2023
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravailEtBordDMS_SimaoHenriquesDaSilva.xlsx
+++ b/Documentation/JournalDeTravailEtBordDMS_SimaoHenriquesDaSilva.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simao.HENRIQUES-SILV\Documents\GitHub\ProjetWebDMS\ProjetWebDMS\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcos.VALENTE-DA-SI\Documents\GitHub\ProjetWebDMS\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="86">
   <si>
     <t>Nom du Projet :</t>
   </si>
@@ -271,6 +271,18 @@
   </si>
   <si>
     <t>Simão Henriques da Silva, Marcos Valente da Silva et Diego Pinto Tomaz</t>
+  </si>
+  <si>
+    <t>Finalisation de la page pour les produits, sans panier</t>
+  </si>
+  <si>
+    <t>Simão Henriques da Silva, Diego Pinto Tomaz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code du login </t>
+  </si>
+  <si>
+    <t>Finalisation de la page login</t>
   </si>
 </sst>
 </file>
@@ -826,13 +838,43 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -858,36 +900,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1493,8 +1505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N9999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="F22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1516,27 +1528,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
     </row>
     <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.25">
       <c r="F2" s="17"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
     </row>
     <row r="3" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F3" s="18"/>
@@ -1544,14 +1556,14 @@
       <c r="H3" s="18"/>
     </row>
     <row r="4" spans="2:14" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="40" t="s">
+      <c r="C4" s="45"/>
+      <c r="D4" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="41"/>
+      <c r="E4" s="51"/>
       <c r="G4" s="20" t="s">
         <v>1</v>
       </c>
@@ -1578,14 +1590,14 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="38" t="s">
+      <c r="C5" s="40"/>
+      <c r="D5" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="39"/>
+      <c r="E5" s="49"/>
       <c r="G5" s="4">
         <v>44957</v>
       </c>
@@ -1613,14 +1625,14 @@
       </c>
     </row>
     <row r="6" spans="2:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="36">
+      <c r="C6" s="40"/>
+      <c r="D6" s="46">
         <v>44957</v>
       </c>
-      <c r="E6" s="37"/>
+      <c r="E6" s="47"/>
       <c r="G6" s="4">
         <v>44957</v>
       </c>
@@ -1648,15 +1660,15 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="50">
+      <c r="C7" s="38"/>
+      <c r="D7" s="41">
         <f>SUM(Tableau1[Durée])</f>
-        <v>1.218055555555555</v>
-      </c>
-      <c r="E7" s="51"/>
+        <v>1.343055555555555</v>
+      </c>
+      <c r="E7" s="42"/>
       <c r="G7" s="4">
         <v>44957</v>
       </c>
@@ -1712,10 +1724,10 @@
     </row>
     <row r="9" spans="2:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="16"/>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="43"/>
+      <c r="D9" s="32"/>
       <c r="G9" s="4">
         <v>44959</v>
       </c>
@@ -1746,10 +1758,10 @@
       <c r="B10" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="45"/>
+      <c r="D10" s="34"/>
       <c r="G10" s="4">
         <v>44959</v>
       </c>
@@ -1780,10 +1792,10 @@
       <c r="B11" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="47"/>
+      <c r="D11" s="36"/>
       <c r="G11" s="4">
         <v>44959</v>
       </c>
@@ -2458,7 +2470,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="7:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="7:14" ht="45" x14ac:dyDescent="0.25">
       <c r="G36" s="4">
         <v>45006</v>
       </c>
@@ -2482,7 +2494,7 @@
         <v>76</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="7:14" ht="30" x14ac:dyDescent="0.25">
@@ -2490,14 +2502,14 @@
         <v>45007</v>
       </c>
       <c r="H37" s="5">
-        <v>0.67361111111111116</v>
+        <v>0.5625</v>
       </c>
       <c r="I37" s="6">
         <v>0.70138888888888884</v>
       </c>
       <c r="J37" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>2.7777777777777679E-2</v>
+        <v>0.13888888888888884</v>
       </c>
       <c r="K37" s="7" t="s">
         <v>22</v>
@@ -2520,11 +2532,11 @@
         <v>0.5625</v>
       </c>
       <c r="I38" s="6">
-        <v>0.70138888888888884</v>
+        <v>0.62847222222222221</v>
       </c>
       <c r="J38" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>0.13888888888888884</v>
+        <v>6.597222222222221E-2</v>
       </c>
       <c r="K38" s="7" t="s">
         <v>22</v>
@@ -2539,44 +2551,86 @@
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G39" s="4"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="6"/>
+    <row r="39" spans="7:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="G39" s="4">
+        <v>45008</v>
+      </c>
+      <c r="H39" s="5">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="I39" s="6">
+        <v>0.70138888888888884</v>
+      </c>
       <c r="J39" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>0</v>
-      </c>
-      <c r="K39" s="7"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
-    </row>
-    <row r="40" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G40" s="4"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="6"/>
+        <v>2.7777777777777679E-2</v>
+      </c>
+      <c r="K39" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L39" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="7:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="G40" s="4">
+        <v>45012</v>
+      </c>
+      <c r="H40" s="5">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I40" s="6">
+        <v>0.36458333333333331</v>
+      </c>
       <c r="J40" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>0</v>
-      </c>
-      <c r="K40" s="7"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
-    </row>
-    <row r="41" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G41" s="4"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="6"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="K40" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L40" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="7:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="G41" s="4">
+        <v>45013</v>
+      </c>
+      <c r="H41" s="5">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="I41" s="6">
+        <v>0.70138888888888884</v>
+      </c>
       <c r="J41" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>0</v>
-      </c>
-      <c r="K41" s="7"/>
-      <c r="L41" s="8"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
+        <v>2.7777777777777679E-2</v>
+      </c>
+      <c r="K41" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L41" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="42" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G42" s="4"/>
@@ -44734,18 +44788,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:N2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D4:E4"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D7:E7"/>
-    <mergeCell ref="G1:N2"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D4:E4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1"/>
@@ -45112,12 +45166,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -45291,15 +45342,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE66B988-21FD-4E82-857E-C2E9A6618F3F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D38AEF9-57C3-439A-B892-EB0F14AB4CC0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="9b42e094-9454-4e38-a519-f9a276a20d04"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -45323,17 +45385,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D38AEF9-57C3-439A-B892-EB0F14AB4CC0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE66B988-21FD-4E82-857E-C2E9A6618F3F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="9b42e094-9454-4e38-a519-f9a276a20d04"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Mise à jour de la documentation.
Mise à jour de la documentation avec la mise à jour dujournal de travail également
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravailEtBordDMS_SimaoHenriquesDaSilva.xlsx
+++ b/Documentation/JournalDeTravailEtBordDMS_SimaoHenriquesDaSilva.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="95">
   <si>
     <t>Nom du Projet :</t>
   </si>
@@ -307,6 +307,9 @@
   </si>
   <si>
     <t>Mise à jour des fichiers sur l'hébergeur</t>
+  </si>
+  <si>
+    <t>Mise à jour de la documentation</t>
   </si>
 </sst>
 </file>
@@ -862,13 +865,43 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -894,36 +927,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1530,7 +1533,7 @@
   <dimension ref="B1:N9999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N47" sqref="N47"/>
+      <selection activeCell="P46" sqref="P46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1552,27 +1555,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
     </row>
     <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.25">
       <c r="F2" s="17"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
     </row>
     <row r="3" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F3" s="18"/>
@@ -1580,14 +1583,14 @@
       <c r="H3" s="18"/>
     </row>
     <row r="4" spans="2:14" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="40" t="s">
+      <c r="C4" s="45"/>
+      <c r="D4" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="41"/>
+      <c r="E4" s="51"/>
       <c r="G4" s="20" t="s">
         <v>1</v>
       </c>
@@ -1614,14 +1617,14 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="38" t="s">
+      <c r="C5" s="40"/>
+      <c r="D5" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="39"/>
+      <c r="E5" s="49"/>
       <c r="G5" s="4">
         <v>44957</v>
       </c>
@@ -1649,14 +1652,14 @@
       </c>
     </row>
     <row r="6" spans="2:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="36">
+      <c r="C6" s="40"/>
+      <c r="D6" s="46">
         <v>44957</v>
       </c>
-      <c r="E6" s="37"/>
+      <c r="E6" s="47"/>
       <c r="G6" s="4">
         <v>44957</v>
       </c>
@@ -1684,15 +1687,15 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="50">
+      <c r="C7" s="38"/>
+      <c r="D7" s="41">
         <f>SUM(Tableau1[Durée])</f>
-        <v>1.5166666666666662</v>
-      </c>
-      <c r="E7" s="51"/>
+        <v>1.5270833333333329</v>
+      </c>
+      <c r="E7" s="42"/>
       <c r="G7" s="4">
         <v>44957</v>
       </c>
@@ -1748,10 +1751,10 @@
     </row>
     <row r="9" spans="2:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="16"/>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="43"/>
+      <c r="D9" s="32"/>
       <c r="G9" s="4">
         <v>44959</v>
       </c>
@@ -1782,10 +1785,10 @@
       <c r="B10" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="45"/>
+      <c r="D10" s="34"/>
       <c r="G10" s="4">
         <v>44959</v>
       </c>
@@ -1816,10 +1819,10 @@
       <c r="B11" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="47"/>
+      <c r="D11" s="36"/>
       <c r="G11" s="4">
         <v>44959</v>
       </c>
@@ -2764,18 +2767,32 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G46" s="4"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="6"/>
+    <row r="46" spans="7:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="G46" s="4">
+        <v>45016</v>
+      </c>
+      <c r="H46" s="5">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="I46" s="6">
+        <v>0.47569444444444442</v>
+      </c>
       <c r="J46" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>0</v>
-      </c>
-      <c r="K46" s="7"/>
-      <c r="L46" s="8"/>
-      <c r="M46" s="1"/>
-      <c r="N46" s="1"/>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="K46" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L46" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="47" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G47" s="4"/>
@@ -44868,18 +44885,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:N2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D4:E4"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D7:E7"/>
-    <mergeCell ref="G1:N2"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D4:E4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1"/>
@@ -45246,12 +45263,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -45425,15 +45439,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE66B988-21FD-4E82-857E-C2E9A6618F3F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D38AEF9-57C3-439A-B892-EB0F14AB4CC0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="9b42e094-9454-4e38-a519-f9a276a20d04"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -45457,17 +45482,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D38AEF9-57C3-439A-B892-EB0F14AB4CC0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE66B988-21FD-4E82-857E-C2E9A6618F3F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="9b42e094-9454-4e38-a519-f9a276a20d04"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>